<commit_message>
dodalem pelny projekt w folderze 4
</commit_message>
<xml_diff>
--- a/PracaNaLekcjiNr4/zadanie 3/tabelka.xlsx
+++ b/PracaNaLekcjiNr4/zadanie 3/tabelka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karol\OneDrive\Pulpit\Szczecin\szkoła\INF\SCI_INF\PracaNaLekcjiNr4\zadanie 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0AE56E5-BCF1-4651-BF5F-4F35036D9457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A35D043-96A6-4E40-8DCD-B981DD75418D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{41714FDC-95C1-4CB1-89E9-EBB079F340BB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Sortowanie</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>różnica</t>
+  </si>
+  <si>
+    <t>wniosek: najlepsze jest sortowanie szybkie</t>
+  </si>
+  <si>
+    <t>przy 1000 elementach losowanie szybkie jest ponad 200 razy szybsze od najwolniejszego sortowania bąbelkowego</t>
+  </si>
+  <si>
+    <t>przy 10000 elementach losowanie szybkie jest ponad 700 razy szybsze od najwolniejszego sortowania bąbelkowego</t>
   </si>
 </sst>
 </file>
@@ -137,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -159,6 +168,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,15 +489,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA4B25D4-6D70-4405-8F48-617EA9A4608E}">
-  <dimension ref="B2:I12"/>
+  <dimension ref="B2:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
     <col min="5" max="5" width="15.44140625" customWidth="1"/>
@@ -712,7 +727,32 @@
         <v>717.27010166358593</v>
       </c>
     </row>
+    <row r="15" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:G16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>